<commit_message>
Changed unit: m to cm
</commit_message>
<xml_diff>
--- a/backend/backend/tests/sample/description.xlsx
+++ b/backend/backend/tests/sample/description.xlsx
@@ -279,19 +279,19 @@
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -602,7 +602,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,10 +615,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -629,79 +629,79 @@
       <c r="F1" s="16"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="8">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="11">
         <v>0</v>
       </c>
-      <c r="F3" s="9">
-        <v>1.45</v>
+      <c r="F3" s="12">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
-        <v>1.45</v>
-      </c>
-      <c r="F4" s="9">
-        <v>3.54</v>
+      <c r="E4" s="11">
+        <v>140</v>
+      </c>
+      <c r="F4" s="12">
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="2">
-        <v>3.54</v>
-      </c>
-      <c r="F5" s="9">
-        <v>5.85</v>
+      <c r="E5" s="11">
+        <v>300</v>
+      </c>
+      <c r="F5" s="12">
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="13">
-        <v>5.85</v>
+        <v>410</v>
       </c>
       <c r="F6" s="14">
-        <v>5.93</v>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>